<commit_message>
working on Arduino code for LightPlay2a
</commit_message>
<xml_diff>
--- a/layouts/lightplay2/lightplay2-BillOfMaterials.xlsx
+++ b/layouts/lightplay2/lightplay2-BillOfMaterials.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="123">
   <si>
     <t>10 uH inductor</t>
   </si>
@@ -385,6 +385,9 @@
   </si>
   <si>
     <t>710-744025100</t>
+  </si>
+  <si>
+    <t>594-5073NW5R600J</t>
   </si>
 </sst>
 </file>
@@ -487,7 +490,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="181">
+  <cellStyleXfs count="183">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -632,6 +635,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -720,7 +725,7 @@
     <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="181">
+  <cellStyles count="183">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -832,6 +837,7 @@
     <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
@@ -901,6 +907,7 @@
     <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1230,10 +1237,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1694,7 +1701,7 @@
         <v>3</v>
       </c>
       <c r="J16" s="6">
-        <f t="shared" ref="J16:J26" si="1">I16*H16</f>
+        <f t="shared" ref="J16:J27" si="1">I16*H16</f>
         <v>1.0499999999999998</v>
       </c>
     </row>
@@ -1792,247 +1799,257 @@
       </c>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>97</v>
-      </c>
+      <c r="C20" s="9"/>
       <c r="F20" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="G20" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="I20" s="18"/>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G21" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="H20" s="6">
+      <c r="H21" s="6">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="I20" s="18">
+      <c r="I21" s="18">
         <v>1</v>
       </c>
-      <c r="J20" s="6">
+      <c r="J21" s="6">
         <f t="shared" si="1"/>
         <v>2.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
-      <c r="A21" s="4" t="s">
+    <row r="22" spans="1:10">
+      <c r="A22" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B22" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C22" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D22" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E22" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="F22" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G21" s="4" t="s">
+      <c r="G22" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="H21" s="6">
+      <c r="H22" s="6">
         <v>1.6E-2</v>
       </c>
-      <c r="I21" s="18">
+      <c r="I22" s="18">
         <v>1</v>
       </c>
-      <c r="J21" s="6">
+      <c r="J22" s="6">
         <f t="shared" si="1"/>
         <v>1.6E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
-      <c r="A22" s="4" t="s">
+    <row r="23" spans="1:10">
+      <c r="A23" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B23" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C23" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D23" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E23" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="F23" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G22" s="4" t="s">
+      <c r="G23" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="H22" s="6">
+      <c r="H23" s="6">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="I22" s="18">
+      <c r="I23" s="18">
         <v>2</v>
       </c>
-      <c r="J22" s="6">
+      <c r="J23" s="6">
         <f t="shared" si="1"/>
         <v>5.6000000000000001E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
-      <c r="A23" s="4" t="s">
+    <row r="24" spans="1:10">
+      <c r="A24" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B24" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C24" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D24" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="E24" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="F24" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G23" s="4" t="s">
+      <c r="G24" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="H23" s="6">
+      <c r="H24" s="6">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="I23" s="18">
+      <c r="I24" s="18">
         <v>3</v>
       </c>
-      <c r="J23" s="6">
+      <c r="J24" s="6">
         <f t="shared" si="1"/>
         <v>8.4000000000000005E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
-      <c r="A24" s="4" t="s">
+    <row r="25" spans="1:10">
+      <c r="A25" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B25" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C25" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D25" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="E24" s="5">
+      <c r="E25" s="5">
         <v>1206</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="F25" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G24" s="12" t="s">
+      <c r="G25" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="H24" s="6">
+      <c r="H25" s="6">
         <v>1.62</v>
       </c>
-      <c r="I24" s="18">
+      <c r="I25" s="18">
         <v>1</v>
       </c>
-      <c r="J24" s="6">
+      <c r="J25" s="6">
         <f t="shared" si="1"/>
         <v>1.62</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
-      <c r="A25" s="4" t="s">
+    <row r="26" spans="1:10">
+      <c r="A26" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B26" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C26" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D26" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="E25" s="5">
+      <c r="E26" s="5">
         <v>1206</v>
       </c>
-      <c r="F25" s="4" t="s">
+      <c r="F26" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G25" s="12" t="s">
+      <c r="G26" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="H25" s="6">
+      <c r="H26" s="6">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="I25" s="18">
+      <c r="I26" s="18">
         <v>1</v>
       </c>
-      <c r="J25" s="6">
+      <c r="J26" s="6">
         <f t="shared" si="1"/>
         <v>5.6000000000000001E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
-      <c r="A26" s="4" t="s">
+    <row r="27" spans="1:10">
+      <c r="A27" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B27" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C27" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D27" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="E26" s="5">
+      <c r="E27" s="5">
         <v>1206</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="F27" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G26" s="12" t="s">
+      <c r="G27" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="H26" s="6">
+      <c r="H27" s="6">
         <v>0.10199999999999999</v>
       </c>
-      <c r="I26" s="18">
+      <c r="I27" s="18">
         <v>1</v>
       </c>
-      <c r="J26" s="6">
+      <c r="J27" s="6">
         <f t="shared" si="1"/>
         <v>0.10199999999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
-      <c r="G28" s="21" t="s">
+    <row r="29" spans="1:10">
+      <c r="G29" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="H28" s="22">
-        <f>SUM(H2:H26)</f>
+      <c r="H29" s="22">
+        <f>SUM(H2:H27)</f>
         <v>52.037999999999997</v>
       </c>
-      <c r="I28" s="22"/>
-      <c r="J28" s="22">
-        <f>SUM(J2:J26)</f>
+      <c r="I29" s="22"/>
+      <c r="J29" s="22">
+        <f>SUM(J2:J27)</f>
         <v>59.231999999999999</v>
       </c>
     </row>

</xml_diff>